<commit_message>
US2: Casos de prueba completados
</commit_message>
<xml_diff>
--- a/Producto/Web/Casos de prueba/6.xlsx
+++ b/Producto/Web/Casos de prueba/6.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="6810" yWindow="315" windowWidth="14805" windowHeight="7950" activeTab="3"/>
+    <workbookView xWindow="6810" yWindow="315" windowWidth="14805" windowHeight="7950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DatosGenerales" sheetId="1" r:id="rId1"/>
@@ -97,10 +97,10 @@
     <t>Ingreso &lt;Ciudad1&gt; en el campo nombre de ciudad</t>
   </si>
   <si>
-    <t>Se carga la pagina BuscarPlayas, con todas las playas de &lt;Ciudad1&gt; disponibles en un mapa.</t>
-  </si>
-  <si>
     <t>Leonel Romero [autor]</t>
+  </si>
+  <si>
+    <t>Se carga la pagina BuscarPlayas, con todas las playas de &lt;Ciudad1&gt; disponibles en un mapa. Se carga la informacion de las playas en la grilla de playas debajo del mapa.</t>
   </si>
 </sst>
 </file>
@@ -700,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -745,7 +745,7 @@
       <c r="C3" s="8"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="25.5">
+    <row r="4" spans="1:4" ht="51">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -753,7 +753,7 @@
         <v>19</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -769,7 +769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -809,7 +809,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>18</v>

</xml_diff>